<commit_message>
Extracted hydro catchment data from climate update PDF
</commit_message>
<xml_diff>
--- a/extracted_data/hydro_catchment_data.xlsx
+++ b/extracted_data/hydro_catchment_data.xlsx
@@ -5141,7 +5141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5150,61 +5150,122 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>01/07/2025</t>
         </is>
       </c>
-      <c r="B1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N1" t="inlineStr">
+      <c r="B1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>(Rathnapura)</t>
         </is>
       </c>
-      <c r="O1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
+      <c r="O1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01/07/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>(Rathnapura)</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>

</xml_diff>